<commit_message>
After practice presentation #1
</commit_message>
<xml_diff>
--- a/data/Observations_Calcs.xlsx
+++ b/data/Observations_Calcs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhanuyerra/Documents/MetisDatScienceBootcamp/Projects/Metis_Prj5/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5275E85B-BFF5-ED40-8F97-826E924225E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3CDC53-95AB-C447-B163-E63EC485E5FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="460" windowWidth="15420" windowHeight="16200" xr2:uid="{A13D65D2-C581-5642-AD6E-C20A950BEB35}"/>
+    <workbookView xWindow="4940" yWindow="460" windowWidth="15420" windowHeight="16200" activeTab="1" xr2:uid="{A13D65D2-C581-5642-AD6E-C20A950BEB35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,9 +32,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="4">
   <si>
     <t>Video1: "4nHElVbT3HY.mp4"</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>has</t>
+  </si>
+  <si>
+    <t>frames</t>
   </si>
 </sst>
 </file>
@@ -416,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA062FC-6D05-1D46-8EE1-B54E7170A3FE}">
   <dimension ref="A3:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,7 +565,7 @@
         <v>1024</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="3"/>
+        <f>FLOOR((G7-48-1)/2,1)</f>
         <v>487</v>
       </c>
       <c r="I7" s="5">
@@ -2395,16 +2405,1992 @@
         <v>73872</v>
       </c>
       <c r="G61">
-        <f t="shared" si="2"/>
+        <f>(F61-E61)/3</f>
         <v>664</v>
       </c>
       <c r="H61">
-        <f t="shared" si="3"/>
+        <f>FLOOR((G61-48-1)/2,1)</f>
         <v>307</v>
       </c>
       <c r="I61" s="2">
         <f t="shared" si="4"/>
         <v>1.3833333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546F8177-C7F1-EA46-A0E7-558FB46960FE}">
+  <dimension ref="A1:I72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>749</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <f>INT(D1/(8*5))</f>
+        <v>18</v>
+      </c>
+      <c r="G1">
+        <f>F1*5</f>
+        <v>90</v>
+      </c>
+      <c r="I1" s="4">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>690</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F65" si="0">INT(D2/(8*5))</f>
+        <v>17</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G65" si="1">F2*5</f>
+        <v>85</v>
+      </c>
+      <c r="I2" s="4">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>653</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="I3" s="4">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1003</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>854</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="I5" s="4">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>629</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="I6" s="4">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>575</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="I7" s="4">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>809</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="I8" s="4">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>766</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="I10" s="4">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>619</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>699</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>566</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>907</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>681</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>112</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>465</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>200</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>164</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>509</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>642</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>664</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>668</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>887</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>809</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>1080</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>666</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>657</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>819</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>663</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>728</v>
+      </c>
+      <c r="E36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>885</v>
+      </c>
+      <c r="E37" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>41</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>535</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>68</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>761</v>
+      </c>
+      <c r="E41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="H41">
+        <f>IF(D41&gt;100, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>75</v>
+      </c>
+      <c r="E42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H42">
+        <f t="shared" ref="H42:H72" si="2">IF(D42&gt;100, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>475</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>224</v>
+      </c>
+      <c r="E44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>45</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>406</v>
+      </c>
+      <c r="E45" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>566</v>
+      </c>
+      <c r="E46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>222</v>
+      </c>
+      <c r="E47" t="s">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>48</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>738</v>
+      </c>
+      <c r="E48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>49</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>792</v>
+      </c>
+      <c r="E49" t="s">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>50</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>761</v>
+      </c>
+      <c r="E50" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>51</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>130</v>
+      </c>
+      <c r="E51" t="s">
+        <v>3</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>52</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>447</v>
+      </c>
+      <c r="E52" t="s">
+        <v>3</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>53</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>585</v>
+      </c>
+      <c r="E53" t="s">
+        <v>3</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>54</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>357</v>
+      </c>
+      <c r="E54" t="s">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>55</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>508</v>
+      </c>
+      <c r="E55" t="s">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>56</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>3</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>57</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>61</v>
+      </c>
+      <c r="E57" t="s">
+        <v>3</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>58</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>667</v>
+      </c>
+      <c r="E58" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>59</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <v>156</v>
+      </c>
+      <c r="E59" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>60</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>783</v>
+      </c>
+      <c r="E60" t="s">
+        <v>3</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>61</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>564</v>
+      </c>
+      <c r="E61" t="s">
+        <v>3</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>62</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>201</v>
+      </c>
+      <c r="E62" t="s">
+        <v>3</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>63</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>474</v>
+      </c>
+      <c r="E63" t="s">
+        <v>3</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>64</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>616</v>
+      </c>
+      <c r="E64" t="s">
+        <v>3</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>65</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>586</v>
+      </c>
+      <c r="E65" t="s">
+        <v>3</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>66</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>730</v>
+      </c>
+      <c r="E66" t="s">
+        <v>3</v>
+      </c>
+      <c r="F66">
+        <f t="shared" ref="F66:F72" si="3">INT(D66/(8*5))</f>
+        <v>18</v>
+      </c>
+      <c r="G66">
+        <f t="shared" ref="G66:G72" si="4">F66*5</f>
+        <v>90</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>67</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>361</v>
+      </c>
+      <c r="E67" t="s">
+        <v>3</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>68</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>384</v>
+      </c>
+      <c r="E68" t="s">
+        <v>3</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>69</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>374</v>
+      </c>
+      <c r="E69" t="s">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>70</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>89</v>
+      </c>
+      <c r="E70" t="s">
+        <v>3</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>71</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <v>763</v>
+      </c>
+      <c r="E71" t="s">
+        <v>3</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>72</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <v>109</v>
+      </c>
+      <c r="E72" t="s">
+        <v>3</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>